<commit_message>
Add columns to event participants Excel list
</commit_message>
<xml_diff>
--- a/lib/assets/event_participants_template.xlsx
+++ b/lib/assets/event_participants_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaw\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABE9BF4-6E60-46DE-B437-9DC93FC74BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202BE2CC-46B6-43CB-A596-F206AD0563D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17010" yWindow="9810" windowWidth="25485" windowHeight="15825" xr2:uid="{8FF6E26D-0BBF-4D28-83FA-8B01315A9C15}"/>
+    <workbookView xWindow="3990" yWindow="9960" windowWidth="25485" windowHeight="15825" xr2:uid="{8FF6E26D-0BBF-4D28-83FA-8B01315A9C15}"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>イベント名</t>
     <rPh sb="4" eb="5">
@@ -131,7 +131,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>as of</t>
+    <t>西暦</t>
+    <rPh sb="0" eb="2">
+      <t>セイレキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>よみがな</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -187,7 +194,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -208,9 +215,6 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,39 +530,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4440D6DF-8E85-4460-8609-412DE745F6EB}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.75" customWidth="1"/>
-    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.25" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -566,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -574,37 +580,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="F10" s="1"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>